<commit_message>
Further changes to FreeCAD files
</commit_message>
<xml_diff>
--- a/content/rigel96/CAD resources/Rigel spreadsheet.xlsx
+++ b/content/rigel96/CAD resources/Rigel spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicholasWilson\Source\keyboards\02-keyopatra-project\CAD resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicholasWilson\Source\keyboards\content\rigel96\CAD resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CB4B26-D37B-460E-96EF-4C743ADC0F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4727F1C7-620A-4273-9D44-814693B3D175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="5510" windowWidth="28800" windowHeight="15370" activeTab="3" xr2:uid="{32EE4ECE-299D-4BED-919A-5106D64CC162}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15370" xr2:uid="{32EE4ECE-299D-4BED-919A-5106D64CC162}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
   <si>
     <t>Thoughts on metals for keyboard plate</t>
   </si>
@@ -362,6 +362,27 @@
   </si>
   <si>
     <t>Radius:</t>
+  </si>
+  <si>
+    <t>Quality Planed Timber Merchants in the UK | Timbersource</t>
+  </si>
+  <si>
+    <t>Ash</t>
+  </si>
+  <si>
+    <t>Beech</t>
+  </si>
+  <si>
+    <t>Maple</t>
+  </si>
+  <si>
+    <t>Meranti</t>
+  </si>
+  <si>
+    <t>American Oak</t>
+  </si>
+  <si>
+    <t>Tulipwood</t>
   </si>
 </sst>
 </file>
@@ -432,11 +453,11 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -799,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7E0C16-8865-409D-A480-46129CE2CEEA}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -814,12 +835,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -931,10 +952,10 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
@@ -944,19 +965,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="1">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -964,11 +1038,14 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B23" r:id="rId1" display="https://www.timbersource.co.uk/planed-timber" xr:uid="{160D0327-ADA8-4F28-8A21-FAFDFB24B7D7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1248,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15110F8F-67DA-46BD-B8B2-C9615236E7CE}">
   <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -1329,14 +1406,14 @@
       <c r="E12" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f>15*PI()/180</f>
         <v>0.26179938779914941</v>
       </c>
       <c r="G12" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <f>C4/2/SIN(F12/2)</f>
         <v>72.973859407022218</v>
       </c>

</xml_diff>